<commit_message>
added data driven tests
</commit_message>
<xml_diff>
--- a/src/test/java/com/heroku/qa/testdata/DataSheet.xlsx
+++ b/src/test/java/com/heroku/qa/testdata/DataSheet.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\girishn3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\girishn3\eclipse-workspace\HerokuProject\src\test\java\com\heroku\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76F9175-8A6E-4E09-958C-D46600A3E98C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D77414-928A-4440-9132-68FE61C3277A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7050" xr2:uid="{27AEC321-5F54-4750-8CAF-27817C5DFF17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7050" activeTab="2" xr2:uid="{27AEC321-5F54-4750-8CAF-27817C5DFF17}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit" sheetId="2" r:id="rId2"/>
+    <sheet name="Delete" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Intro Date</t>
   </si>
@@ -73,6 +75,9 @@
   </si>
   <si>
     <t>2021-06-10</t>
+  </si>
+  <si>
+    <t>new company</t>
   </si>
 </sst>
 </file>
@@ -427,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6246C826-3152-44A4-99A8-D05325BFCCAB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,4 +503,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D36B80F-0718-4B8A-90BB-F745187B597C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A27FD12-6C73-49D2-97D7-9A36CA9CBA69}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>